<commit_message>
tests pass and catch worker exceptions
</commit_message>
<xml_diff>
--- a/pyomrx/tests/res/exam_form/example_exam_form.xlsx
+++ b/pyomrx/tests/res/exam_form/example_exam_form.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="circles_code" comment="row fill: one, column prefix:c_">template!$C$5:$L$8</definedName>
-    <definedName name="circles_scores" comment="row fill: one column prefix: none">template!$C$10:$L$35</definedName>
+    <definedName name="circles_scores" comment="row fill: one, column prefix: none">template!$C$10:$L$35</definedName>
     <definedName name="meta_paper_code">template!$AL$7:$AL$9</definedName>
     <definedName name="page_1">template!$A$1:$AN$36</definedName>
     <definedName name="sub_form_1">template!$B$2:$L$35</definedName>
@@ -601,7 +601,7 @@
   <dimension ref="A1:AN36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ10" sqref="AJ10"/>
+      <selection activeCell="AO16" sqref="AO16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
readme, cli and other open source prep (#31)
* add examples with tests2

* cli

* cleanup test resources

* more test resources

* cleanup

* readme and license

* entry point and setup improvements

* give up on pypi for now

* cleanup

* remove abortable comment

* cleanup

* yapf
</commit_message>
<xml_diff>
--- a/pyomrx/tests/res/exam_form/example_exam_form.xlsx
+++ b/pyomrx/tests/res/exam_form/example_exam_form.xlsx
@@ -15,8 +15,8 @@
     <sheet name="template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="circles_code" comment="row fill: one, column prefix:c_">template!$C$5:$L$8</definedName>
-    <definedName name="circles_scores" comment="row fill: one, column prefix: none">template!$C$10:$L$35</definedName>
+    <definedName name="circles_code" comment="row fill: one, column prefix:C">template!$C$5:$L$8</definedName>
+    <definedName name="circles_scores" comment="row fill: one, column prefix: A">template!$C$10:$L$35</definedName>
     <definedName name="meta_paper_code">template!$AL$7:$AL$9</definedName>
     <definedName name="page_1">template!$A$1:$AN$36</definedName>
     <definedName name="sub_form_1">template!$B$2:$L$35</definedName>

</xml_diff>